<commit_message>
trgnati temp files, slika od excel dodadeno
</commit_message>
<xml_diff>
--- a/EveryStatementTests.xlsx
+++ b/EveryStatementTests.xlsx
@@ -32,10 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="48">
-  <si>
-    <t>Node</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="35">
   <si>
     <t>Source Line</t>
   </si>
@@ -59,42 +56,6 @@
   </si>
   <si>
     <t>email</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>L</t>
   </si>
   <si>
     <r>
@@ -793,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -809,359 +770,333 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="1" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="2:17" ht="14.25" customHeight="1">
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="3" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="O3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:17" ht="15" customHeight="1">
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="B4" s="2"/>
       <c r="C4" s="3" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="P4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="2:17">
-      <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="B5" s="2"/>
       <c r="C5" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="P5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q5" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="2:17">
-      <c r="B6" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="B6" s="2"/>
       <c r="C6" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="M6" s="6"/>
       <c r="P6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:17">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="2"/>
+      <c r="C7" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="2:17">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="2"/>
+      <c r="C8" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="K8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O8" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="2:17">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="L9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M9" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="P9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q9" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:17">
-      <c r="B10" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="B10" s="2"/>
       <c r="C10" s="4" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F10" s="2"/>
       <c r="L10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M10" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="P10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q10" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="2:17">
-      <c r="B11" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="B11" s="2"/>
       <c r="C11" s="4" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="L11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="P11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="2:17">
-      <c r="B12" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="B12" s="2"/>
       <c r="C12" s="3" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="2:17">
-      <c r="B13" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="B13" s="2"/>
       <c r="C13" s="3" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="K13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="2:17">
-      <c r="B14" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="B14" s="2"/>
       <c r="C14" s="3" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="L14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M14" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:17">
@@ -1171,10 +1106,10 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="L15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M15" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="2:17">
@@ -1184,10 +1119,10 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="L16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="2:17">

</xml_diff>